<commit_message>
Completed Course, added certificate
</commit_message>
<xml_diff>
--- a/Introduction-To-Microsoft-Excel/ACME Company Move.xlsx
+++ b/Introduction-To-Microsoft-Excel/ACME Company Move.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/chiw2_student_unimelb_edu_au/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/chiw2_student_unimelb_edu_au/Documents/Projects/Coursera-Courses/Introduction-To-Microsoft-Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09ACC79E-5732-4290-BA64-BAE3B6AD1FC4}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A7CCA86-AE2B-48F1-A53C-BC590FBCE2DC}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="4800" windowWidth="28335" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="2145" windowWidth="27975" windowHeight="16560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Corporate" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +212,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -221,7 +230,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -229,14 +238,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,239 +578,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>44470</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>44470</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <f>D2+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>10</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>44470</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <f t="shared" ref="D4:D15" si="0">D3+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>15</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>44470</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>44470</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>44470</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>44470</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>9</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>44471</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="4">
         <v>44471</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>6</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="4">
         <v>44471</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>5</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="4">
         <v>44471</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>4</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="4">
         <v>44471</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>12</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="4">
         <v>44471</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>3</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <v>44471</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>SUM(B2:B15)</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>B16+Annex1!B9+Annex2!B9</f>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -794,127 +835,136 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365C0597-6A48-41F6-BF5E-736DFADD704D}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>44477</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>44477</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>44477</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>44477</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>44477</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>44477</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>44477</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f>SUM(B2:B8)</f>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -925,15 +975,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69A4E43-9EA3-4180-8ACE-C7F76CA76017}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -951,103 +1004,109 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>44482</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>44481</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>6</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>44481</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>44481</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>44481</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>7</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>44481</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>8</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>44481</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f>SUM(B2:B8)</f>
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>